<commit_message>
resultados exp 2 ent 1
</commit_message>
<xml_diff>
--- a/JMeter/GraficaEntregaFinal.xlsx
+++ b/JMeter/GraficaEntregaFinal.xlsx
@@ -5,16 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebastiansanchez/IngenieriaSistemas/2017-1/ArquiSoft/Proyecto/musical-octo-happiness/JMeter/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/santiago/Documents/arquisoft/musical-octo-happiness/JMeter/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="20" yWindow="460" windowWidth="28800" windowHeight="16380" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="postMedicion" sheetId="2" r:id="rId2"/>
-    <sheet name="post(50x20)" sheetId="3" r:id="rId3"/>
+    <sheet name="Experimento 2 - Entrega 1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="13">
   <si>
     <t>agregarMedicion</t>
   </si>
@@ -51,15 +51,34 @@
   <si>
     <t>Media (ms)</t>
   </si>
+  <si>
+    <t>Balanceador de carga</t>
+  </si>
+  <si>
+    <t>Nodo único</t>
+  </si>
+  <si>
+    <t>20 ITERACIONES</t>
+  </si>
+  <si>
+    <t># threads</t>
+  </si>
+  <si>
+    <t>Desv. Estandar</t>
+  </si>
+  <si>
+    <t>1 ITERACIÓN</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="6" formatCode="&quot;COP&quot;#,##0_);[Red]\(&quot;COP&quot;#,##0\)"/>
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -90,6 +109,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -114,21 +148,56 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -350,11 +419,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2042154672"/>
-        <c:axId val="2038556736"/>
+        <c:axId val="1006781440"/>
+        <c:axId val="1006785200"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2042154672"/>
+        <c:axId val="1006781440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1200.0"/>
@@ -468,12 +537,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2038556736"/>
+        <c:crossAx val="1006785200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2038556736"/>
+        <c:axId val="1006785200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1200.0"/>
@@ -587,7 +656,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2042154672"/>
+        <c:crossAx val="1006781440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -845,11 +914,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2073885632"/>
-        <c:axId val="2080209808"/>
+        <c:axId val="1007847920"/>
+        <c:axId val="1007851040"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2073885632"/>
+        <c:axId val="1007847920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -962,12 +1031,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2080209808"/>
+        <c:crossAx val="1007851040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2080209808"/>
+        <c:axId val="1007851040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1079,7 +1148,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2073885632"/>
+        <c:crossAx val="1007847920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1341,11 +1410,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2080230464"/>
-        <c:axId val="2080233584"/>
+        <c:axId val="1007875392"/>
+        <c:axId val="1007879152"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2080230464"/>
+        <c:axId val="1007875392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1457,12 +1526,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2080233584"/>
+        <c:crossAx val="1007879152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2080233584"/>
+        <c:axId val="1007879152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1574,7 +1643,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2080230464"/>
+        <c:crossAx val="1007875392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1833,11 +1902,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2040572336"/>
-        <c:axId val="1970444480"/>
+        <c:axId val="1006815264"/>
+        <c:axId val="1006818608"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2040572336"/>
+        <c:axId val="1006815264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1949,12 +2018,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1970444480"/>
+        <c:crossAx val="1006818608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1970444480"/>
+        <c:axId val="1006818608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2066,7 +2135,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2040572336"/>
+        <c:crossAx val="1006815264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2150,7 +2219,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Tiempo Medio de Respuesta</a:t>
+              <a:t>20 iteraciones</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -2189,13 +2258,24 @@
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
-        <c:scatterStyle val="smoothMarker"/>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Experimento 2 - Entrega 1'!$G$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Balanceador de carga</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -2220,10 +2300,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'post(50x20)'!$B$6:$B$16</c:f>
+              <c:f>'Experimento 2 - Entrega 1'!$F$3:$F$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1100.0</c:v>
                 </c:pt>
@@ -2250,10 +2330,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'post(50x20)'!$C$6:$C$16</c:f>
+              <c:f>'Experimento 2 - Entrega 1'!$G$3:$G$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>162.0</c:v>
                 </c:pt>
@@ -2278,7 +2358,107 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="1"/>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Experimento 2 - Entrega 1'!$H$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Nodo único</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Experimento 2 - Entrega 1'!$F$3:$F$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1100.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>900.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>800.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>700.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>600.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>500.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Experimento 2 - Entrega 1'!$H$3:$H$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>138.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>84.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>67.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>51.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>28.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>40.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2288,30 +2468,16 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2075645056"/>
-        <c:axId val="2075676640"/>
+        <c:axId val="1047578256"/>
+        <c:axId val="1008991040"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2075645056"/>
+        <c:axId val="1047578256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -2368,7 +2534,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2377,8 +2543,8 @@
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -2405,12 +2571,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2075676640"/>
+        <c:crossAx val="1008991040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2075676640"/>
+        <c:axId val="1008991040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2451,7 +2617,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>t (ms)</a:t>
+                  <a:t>Media (ms)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -2491,14 +2657,8 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
+          <a:ln>
+            <a:noFill/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -2522,7 +2682,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2075645056"/>
+        <c:crossAx val="1047578256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2534,6 +2694,38 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -2606,11 +2798,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Porcentaje</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> de Error</a:t>
+              <a:t>1 iteración</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -2649,13 +2837,24 @@
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
-        <c:scatterStyle val="smoothMarker"/>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Experimento 2 - Entrega 1'!$G$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Balanceador de carga</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -2680,65 +2879,225 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'post(50x20)'!$B$6:$B$16</c:f>
+              <c:f>'Experimento 2 - Entrega 1'!$F$24:$F$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
+                  <c:v>1200.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>1100.0</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>1000.0</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>900.0</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>800.0</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>700.0</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>600.0</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>400.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>300.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>200.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>100.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'post(50x20)'!$D$6:$D$16</c:f>
+              <c:f>'Experimento 2 - Entrega 1'!$G$24:$G$35</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0" formatCode="General">
-                  <c:v>0.0</c:v>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>923.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>1112.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0</c:v>
+                  <c:v>921.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0</c:v>
+                  <c:v>805.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0</c:v>
+                  <c:v>715.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.0</c:v>
+                  <c:v>867.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.0</c:v>
+                  <c:v>317.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>398.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>305.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>104.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>29.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="1"/>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Experimento 2 - Entrega 1'!$H$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Nodo único</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Experimento 2 - Entrega 1'!$F$24:$F$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1200.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1100.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>900.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>800.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>700.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>600.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>400.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>300.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>200.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>100.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Experimento 2 - Entrega 1'!$H$24:$H$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1169.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>984.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>955.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>942.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>841.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>696.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>243.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>166.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2748,30 +3107,16 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2075546336"/>
-        <c:axId val="2075533296"/>
+        <c:axId val="1007490416"/>
+        <c:axId val="1009823312"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2075546336"/>
+        <c:axId val="1007490416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -2828,6 +3173,7 @@
             </a:p>
           </c:txPr>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2836,8 +3182,8 @@
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -2864,12 +3210,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2075533296"/>
+        <c:crossAx val="1009823312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2075533296"/>
+        <c:axId val="1009823312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2910,7 +3256,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>%</a:t>
+                  <a:t>Media (ms)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -2950,14 +3296,8 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
+          <a:ln>
+            <a:noFill/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -2981,7 +3321,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2075546336"/>
+        <c:crossAx val="1007490416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2993,84 +3333,8 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Throughput</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US" baseline="0"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
+    <c:legend>
+      <c:legendPos val="b"/>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -3085,7 +3349,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -3100,355 +3364,7 @@
           <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="smoothMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'post(50x20)'!$B$6:$B$16</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>1100.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1000.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>900.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>800.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>700.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>600.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>500.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'post(50x20)'!$E$6:$E$16</c:f>
-              <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>18.3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>16.6</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>14.9</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>13.3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>11.6</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>10.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>8.3</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="2076516992"/>
-        <c:axId val="2076519696"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="2076516992"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t># Threads</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="2076519696"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="2076519696"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Threas/seg</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="2076516992"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -3726,46 +3642,6 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -5831,7 +5707,7 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -5858,8 +5734,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -5939,6 +5815,11 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -5949,6 +5830,11 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -5960,7 +5846,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="19050" cap="rnd">
+      <a:ln w="28575" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -5980,6 +5866,9 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -5992,10 +5881,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -6035,23 +5924,22 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -6156,8 +6044,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -6289,20 +6177,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -6316,17 +6203,6 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -6347,7 +6223,7 @@
 </file>
 
 <file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -6374,8 +6250,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -6455,6 +6331,11 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -6465,6 +6346,11 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -6476,7 +6362,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="19050" cap="rnd">
+      <a:ln w="28575" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -6496,6 +6382,9 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -6508,10 +6397,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -6551,23 +6440,22 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -6672,8 +6560,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -6805,20 +6693,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -6832,533 +6719,6 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -7516,23 +6876,21 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>812800</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>431800</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -7548,20 +6906,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>12700</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="6" name="Chart 5"/>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -7573,38 +6931,6 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>165100</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>203200</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -7879,7 +7205,7 @@
   <dimension ref="B1:AA37"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="O18" sqref="O18"/>
+      <selection activeCell="C1" sqref="C1:I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8976,8 +8302,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B5:E18"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9192,152 +8518,882 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B5:E16"/>
+  <dimension ref="A1:M49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+    <sheetView tabSelected="1" topLeftCell="G22" zoomScale="193" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B5" s="2" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="F2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C5" t="s">
+      <c r="G2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D5" t="s">
+      <c r="C3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E5" t="s">
+      <c r="D3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3">
+        <v>1100</v>
+      </c>
+      <c r="G3">
+        <v>162</v>
+      </c>
+      <c r="H3">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1100</v>
+      </c>
+      <c r="B4">
+        <v>162</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4" s="3">
+        <v>18.3</v>
+      </c>
+      <c r="F4" s="2">
+        <v>1000</v>
+      </c>
+      <c r="G4">
+        <v>184</v>
+      </c>
+      <c r="H4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>1000</v>
+      </c>
+      <c r="B5">
+        <v>184</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0</v>
+      </c>
+      <c r="D5" s="3">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="F5">
+        <v>900</v>
+      </c>
+      <c r="G5">
+        <v>161</v>
+      </c>
+      <c r="H5">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>900</v>
+      </c>
+      <c r="B6">
+        <v>161</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0</v>
+      </c>
+      <c r="D6" s="3">
+        <v>14.9</v>
+      </c>
+      <c r="F6" s="2">
+        <v>800</v>
+      </c>
+      <c r="G6">
+        <v>158</v>
+      </c>
+      <c r="H6">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>800</v>
+      </c>
+      <c r="B7">
+        <v>158</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0</v>
+      </c>
+      <c r="D7" s="3">
+        <v>13.3</v>
+      </c>
+      <c r="F7">
+        <v>700</v>
+      </c>
+      <c r="G7">
+        <v>171</v>
+      </c>
+      <c r="H7">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>700</v>
+      </c>
+      <c r="B8">
+        <v>171</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0</v>
+      </c>
+      <c r="D8" s="3">
+        <v>11.6</v>
+      </c>
+      <c r="F8" s="2">
+        <v>600</v>
+      </c>
+      <c r="G8">
+        <v>182</v>
+      </c>
+      <c r="H8">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>600</v>
+      </c>
+      <c r="B9">
+        <v>182</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0</v>
+      </c>
+      <c r="D9" s="3">
+        <v>10</v>
+      </c>
+      <c r="F9">
+        <v>500</v>
+      </c>
+      <c r="G9">
+        <v>170</v>
+      </c>
+      <c r="H9">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>500</v>
+      </c>
+      <c r="B10">
+        <v>170</v>
+      </c>
+      <c r="C10" s="4">
+        <v>0</v>
+      </c>
+      <c r="D10" s="3">
+        <v>8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>1100</v>
+      </c>
+      <c r="B13">
+        <v>138</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13" s="4">
+        <v>61.008854871463299</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A14" s="2">
+        <v>1000</v>
+      </c>
+      <c r="B14">
+        <v>100</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14" s="4">
+        <v>62.999415481415397</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>900</v>
+      </c>
+      <c r="B15">
+        <v>84</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15" s="4">
+        <v>61.624524178665297</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A16" s="2">
+        <v>800</v>
+      </c>
+      <c r="B16">
+        <v>67</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16" s="4">
+        <v>34.515285902589497</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>700</v>
+      </c>
+      <c r="B17">
+        <v>51</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17" s="4">
+        <v>27.217862494610198</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" s="2">
+        <v>600</v>
+      </c>
+      <c r="B18">
+        <v>28</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18" s="4">
+        <v>11.058167419001499</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>500</v>
+      </c>
+      <c r="B19">
+        <v>40</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19" s="4">
+        <v>17.4913211622221</v>
+      </c>
+      <c r="H19" s="9"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" s="7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B6">
+      <c r="F23" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H23" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>1200</v>
+      </c>
+      <c r="B24">
+        <v>923</v>
+      </c>
+      <c r="C24" s="4">
+        <v>31</v>
+      </c>
+      <c r="D24" s="3">
+        <v>331.8</v>
+      </c>
+      <c r="F24">
+        <v>1200</v>
+      </c>
+      <c r="G24">
+        <v>923</v>
+      </c>
+      <c r="H24">
+        <v>1169</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25">
         <v>1100</v>
       </c>
-      <c r="C6">
-        <v>162</v>
-      </c>
-      <c r="D6">
+      <c r="B25">
+        <v>1112</v>
+      </c>
+      <c r="C25">
+        <v>41.18</v>
+      </c>
+      <c r="D25" s="3">
+        <v>18.3</v>
+      </c>
+      <c r="F25">
+        <v>1100</v>
+      </c>
+      <c r="G25">
+        <v>1112</v>
+      </c>
+      <c r="H25">
+        <v>984</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26" s="2">
+        <v>1000</v>
+      </c>
+      <c r="B26">
+        <v>921</v>
+      </c>
+      <c r="C26" s="4">
+        <v>18.7</v>
+      </c>
+      <c r="D26" s="3">
+        <v>301.10000000000002</v>
+      </c>
+      <c r="F26" s="2">
+        <v>1000</v>
+      </c>
+      <c r="G26">
+        <v>921</v>
+      </c>
+      <c r="H26">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>900</v>
+      </c>
+      <c r="B27">
+        <v>805</v>
+      </c>
+      <c r="C27" s="4">
+        <v>4.22</v>
+      </c>
+      <c r="D27" s="3">
+        <v>366.4</v>
+      </c>
+      <c r="F27">
+        <v>900</v>
+      </c>
+      <c r="G27">
+        <v>805</v>
+      </c>
+      <c r="H27">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28" s="2">
+        <v>800</v>
+      </c>
+      <c r="B28">
+        <v>715</v>
+      </c>
+      <c r="C28" s="4">
         <v>0</v>
       </c>
-      <c r="E6" s="3">
-        <v>18.3</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B7" s="2">
+      <c r="D28" s="3">
+        <v>306.39999999999998</v>
+      </c>
+      <c r="F28" s="2">
+        <v>800</v>
+      </c>
+      <c r="G28">
+        <v>715</v>
+      </c>
+      <c r="H28">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>700</v>
+      </c>
+      <c r="B29">
+        <v>867</v>
+      </c>
+      <c r="C29" s="4">
+        <v>1.57</v>
+      </c>
+      <c r="D29" s="3">
+        <v>244.1</v>
+      </c>
+      <c r="F29">
+        <v>700</v>
+      </c>
+      <c r="G29">
+        <v>867</v>
+      </c>
+      <c r="H29">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A30" s="2">
+        <v>600</v>
+      </c>
+      <c r="B30">
+        <v>317</v>
+      </c>
+      <c r="C30" s="4">
+        <v>0</v>
+      </c>
+      <c r="D30" s="3">
+        <v>370.6</v>
+      </c>
+      <c r="F30" s="2">
+        <v>600</v>
+      </c>
+      <c r="G30">
+        <v>317</v>
+      </c>
+      <c r="H30">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>500</v>
+      </c>
+      <c r="B31">
+        <v>398</v>
+      </c>
+      <c r="C31" s="4">
+        <v>0</v>
+      </c>
+      <c r="D31" s="3">
+        <v>124.9</v>
+      </c>
+      <c r="E31" s="7"/>
+      <c r="F31">
+        <v>500</v>
+      </c>
+      <c r="G31">
+        <v>398</v>
+      </c>
+      <c r="H31">
+        <v>166</v>
+      </c>
+      <c r="I31" s="7"/>
+      <c r="J31" s="7"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A32" s="2">
+        <v>400</v>
+      </c>
+      <c r="B32">
+        <v>305</v>
+      </c>
+      <c r="C32" s="4">
+        <v>0</v>
+      </c>
+      <c r="D32" s="3">
+        <v>241.8</v>
+      </c>
+      <c r="F32" s="2">
+        <v>400</v>
+      </c>
+      <c r="G32">
+        <v>305</v>
+      </c>
+      <c r="H32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>300</v>
+      </c>
+      <c r="B33">
+        <v>104</v>
+      </c>
+      <c r="C33" s="4">
+        <v>0</v>
+      </c>
+      <c r="D33" s="3">
+        <v>270</v>
+      </c>
+      <c r="F33">
+        <v>300</v>
+      </c>
+      <c r="G33">
+        <v>104</v>
+      </c>
+      <c r="H33">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A34" s="2">
+        <v>200</v>
+      </c>
+      <c r="B34">
+        <v>29</v>
+      </c>
+      <c r="C34" s="4">
+        <v>0</v>
+      </c>
+      <c r="D34" s="3">
+        <v>179.2</v>
+      </c>
+      <c r="F34" s="2">
+        <v>200</v>
+      </c>
+      <c r="G34">
+        <v>29</v>
+      </c>
+      <c r="H34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>100</v>
+      </c>
+      <c r="B35">
+        <v>12</v>
+      </c>
+      <c r="C35" s="4">
+        <v>0</v>
+      </c>
+      <c r="D35" s="3">
+        <v>97.9</v>
+      </c>
+      <c r="F35">
+        <v>100</v>
+      </c>
+      <c r="G35">
+        <v>12</v>
+      </c>
+      <c r="H35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A36" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A37" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>1200</v>
+      </c>
+      <c r="B38">
+        <v>1169</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38" s="3">
+        <v>305.49898167006103</v>
+      </c>
+      <c r="F38" s="2"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>1100</v>
+      </c>
+      <c r="B39">
+        <v>984</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39" s="3">
+        <v>289.32140978432398</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A40">
         <v>1000</v>
       </c>
-      <c r="C7">
-        <v>184</v>
-      </c>
-      <c r="D7" s="4">
+      <c r="B40">
+        <v>955</v>
+      </c>
+      <c r="C40">
         <v>0</v>
       </c>
-      <c r="E7" s="3">
-        <v>16.600000000000001</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B8">
+      <c r="D40" s="3">
+        <v>286.61507595299503</v>
+      </c>
+      <c r="F40" s="2"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A41">
         <v>900</v>
       </c>
-      <c r="C8">
-        <v>161</v>
-      </c>
-      <c r="D8" s="4">
+      <c r="B41">
+        <v>942</v>
+      </c>
+      <c r="C41">
         <v>0</v>
       </c>
-      <c r="E8" s="3">
-        <v>14.9</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B9" s="2">
+      <c r="D41" s="3">
+        <v>284.270372710044</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A42">
         <v>800</v>
       </c>
-      <c r="C9">
-        <v>158</v>
-      </c>
-      <c r="D9" s="4">
+      <c r="B42">
+        <v>841</v>
+      </c>
+      <c r="C42">
         <v>0</v>
       </c>
-      <c r="E9" s="3">
-        <v>13.3</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B10">
+      <c r="D42" s="3">
+        <v>290.06526468455399</v>
+      </c>
+      <c r="F42" s="2"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A43">
         <v>700</v>
       </c>
-      <c r="C10">
-        <v>171</v>
-      </c>
-      <c r="D10" s="4">
+      <c r="B43">
+        <v>696</v>
+      </c>
+      <c r="C43">
         <v>0</v>
       </c>
-      <c r="E10" s="3">
-        <v>11.6</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B11" s="2">
+      <c r="D43" s="3">
+        <v>297.99914857386102</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A44">
         <v>600</v>
       </c>
-      <c r="C11">
-        <v>182</v>
-      </c>
-      <c r="D11" s="4">
+      <c r="B44">
+        <v>243</v>
+      </c>
+      <c r="C44">
         <v>0</v>
       </c>
-      <c r="E11" s="3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B12">
+      <c r="D44" s="3">
+        <v>308.64197530864197</v>
+      </c>
+      <c r="F44" s="2"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A45">
         <v>500</v>
       </c>
-      <c r="C12">
-        <v>170</v>
-      </c>
-      <c r="D12" s="4">
+      <c r="B45">
+        <v>166</v>
+      </c>
+      <c r="C45">
         <v>0</v>
       </c>
-      <c r="E12" s="3">
-        <v>8.3000000000000007</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B13" s="2"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="3"/>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D14" s="4"/>
-      <c r="E14" s="3"/>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B15" s="2"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="3"/>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D16" s="4"/>
-      <c r="E16" s="3"/>
+      <c r="D45" s="3">
+        <v>318.06615776081401</v>
+      </c>
+      <c r="H45" s="4"/>
+      <c r="I45" s="3"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>400</v>
+      </c>
+      <c r="B46">
+        <v>2</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="D46" s="3">
+        <v>266.31158455392801</v>
+      </c>
+      <c r="F46" s="2"/>
+      <c r="H46" s="4"/>
+      <c r="I46" s="3"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>300</v>
+      </c>
+      <c r="B47">
+        <v>3</v>
+      </c>
+      <c r="C47">
+        <v>0</v>
+      </c>
+      <c r="D47" s="3">
+        <v>294.11764705882302</v>
+      </c>
+      <c r="H47" s="4"/>
+      <c r="I47" s="3"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>200</v>
+      </c>
+      <c r="B48">
+        <v>2</v>
+      </c>
+      <c r="C48">
+        <v>0</v>
+      </c>
+      <c r="D48" s="3">
+        <v>173.91304347825999</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>100</v>
+      </c>
+      <c r="B49">
+        <v>3</v>
+      </c>
+      <c r="C49">
+        <v>0</v>
+      </c>
+      <c r="D49" s="3">
+        <v>87.796312554872699</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A22:D22"/>
+    <mergeCell ref="A36:D36"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A21:D21"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>